<commit_message>
improved spelling in excell sheet
</commit_message>
<xml_diff>
--- a/doc/kosten.xlsx
+++ b/doc/kosten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\project1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\PiTrain\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>ARTIKLE</t>
-  </si>
-  <si>
     <t>sd kaart 64 gb</t>
   </si>
   <si>
@@ -53,15 +50,9 @@
     <t>band kabel 40pins</t>
   </si>
   <si>
-    <t>conector idc</t>
-  </si>
-  <si>
     <t>box header 2x20 man</t>
   </si>
   <si>
-    <t xml:space="preserve">bandcabel 20 cm met 2x conector  </t>
-  </si>
-  <si>
     <t>behuizing rpi</t>
   </si>
   <si>
@@ -89,7 +80,16 @@
     <t>raspberry pi 2</t>
   </si>
   <si>
-    <t>totaal</t>
+    <t>ARTIKEL</t>
+  </si>
+  <si>
+    <t>connector idc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bandkabel 20 cm met 2x conector  </t>
+  </si>
+  <si>
+    <t>TOTAAL</t>
   </si>
 </sst>
 </file>
@@ -125,8 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,158 +421,218 @@
     <col min="3" max="3" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
         <v>4</v>
       </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
         <v>19.989999999999998</v>
       </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="1">
         <v>17.489999999999998</v>
       </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1">
         <v>2.99</v>
       </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1">
         <v>8</v>
       </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="1">
         <v>9</v>
       </c>
-      <c r="D16">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1">
         <v>3</v>
       </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="D20" s="1">
         <v>7</v>
       </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1">
         <v>9.9</v>
       </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1">
         <v>10.8</v>
       </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1">
         <v>2</v>
       </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="D28" s="1">
         <v>1.6</v>
       </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30">
+        <v>13</v>
+      </c>
+      <c r="D30" s="1">
         <v>3.2</v>
       </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1">
         <v>270</v>
       </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35">
+        <v>16</v>
+      </c>
+      <c r="D35" s="1">
         <v>40</v>
       </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38">
+        <v>17</v>
+      </c>
+      <c r="D38" s="1">
         <v>50</v>
       </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>21</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <f>SUM(D3:D38)</f>
         <v>458.97</v>
       </c>

</xml_diff>